<commit_message>
New data analysis done
</commit_message>
<xml_diff>
--- a/data/Top Features.xlsx
+++ b/data/Top Features.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishek.sawalkar/Library/CloudStorage/Box-Box/KrishnanA-RutgersStudents/Sawalkar/bme_analysis/trauma-data-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6762530-54C9-CD48-ACE9-7AF09ED93EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B92EFF1-4B87-B04E-AAAF-6BA08813B4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" activeTab="1" xr2:uid="{890DD962-B85F-9948-A128-9AF0A44C0303}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="19540" activeTab="2" xr2:uid="{890DD962-B85F-9948-A128-9AF0A44C0303}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet6" sheetId="6" r:id="rId1"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId1"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId2"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId3"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId8"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="100">
   <si>
     <t>Ddimer Conc (ng/mL) [Laboratory measurement?]</t>
   </si>
@@ -321,6 +324,27 @@
   </si>
   <si>
     <t>Hemoglobin</t>
+  </si>
+  <si>
+    <t>Ddimer Conc (ug/mL) (Biomedical)</t>
+  </si>
+  <si>
+    <t>Fibrinogen (mg/mL) (Biomedical)</t>
+  </si>
+  <si>
+    <t>Top Features All Updated Data</t>
+  </si>
+  <si>
+    <t>tPA Conc (ng/mL)</t>
+  </si>
+  <si>
+    <t>Top Features - After RFE</t>
+  </si>
+  <si>
+    <t>Intl Normalized Ratio (INR)</t>
+  </si>
+  <si>
+    <t>Top FeaturesRenamed for updated data</t>
   </si>
 </sst>
 </file>
@@ -382,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -412,6 +436,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,11 +750,1753 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD1C70C-9AC8-5441-946F-BAD0F6821D5C}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12.71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10.4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9.64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5.91</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5.41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5.19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5.08</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4.09</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.05</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3.88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3.62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3.59</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3.56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3.38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2.86</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2.82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2.67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2.17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159888AA-A2CB-E149-AEFC-0984670E0D56}">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="37.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0.14888499999999999</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>9.8431000000000005E-2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>5.3726000000000003E-2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>5.2663000000000001E-2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4.7896000000000001E-2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3.7117999999999998E-2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3.4874000000000002E-2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2.9073999999999999E-2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2.8028999999999998E-2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2.6471000000000001E-2</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2.5964000000000001E-2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2.4220999999999999E-2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2.3806000000000001E-2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>2.1336000000000001E-2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.7930000000000001E-2</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1.7385999999999999E-2</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1.4432E-2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1.37E-2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1.3213000000000001E-2</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1.2843E-2</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1.2788000000000001E-2</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1.2095E-2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1.1764E-2</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1.0971E-2</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1.0614999999999999E-2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>9.1190000000000004E-3</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>8.8669999999999999E-3</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>8.7849999999999994E-3</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>8.3149999999999995E-3</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>8.1309999999999993E-3</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>7.7980000000000002E-3</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>7.6969999999999998E-3</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>7.5950000000000002E-3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>7.1310000000000002E-3</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>6.842E-3</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>6.6620000000000004E-3</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>6.5729999999999998E-3</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>6.5319999999999996E-3</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>6.3140000000000002E-3</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>6.2750000000000002E-3</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>6.0010000000000003E-3</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>5.9760000000000004E-3</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>5.7299999999999999E-3</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>5.6559999999999996E-3</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>5.3969999999999999E-3</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>4.7299999999999998E-3</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>4.5139999999999998E-3</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>3.8349999999999999E-3</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>3.7620000000000002E-3</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>3.0990000000000002E-3</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B1790C-9745-9F4A-86FD-4638BE0C1F74}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>13.15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8.07</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7.9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6.9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5.31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3.57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3.02</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2.68</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2.59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2.52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2.17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2.13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2.11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1.99</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1.98</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1.73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1.67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1.56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1.56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F890DE63-AD85-B84E-B48A-90E3C92B935D}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>22.39</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9.07</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6.7</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6.11</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6.01</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5.49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5.19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.07</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3.64</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3.6</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3.39</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3.23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3.05</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3.05</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3.03</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2.83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2.09</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1.36</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1.3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07DDED0-8EB0-1747-9B54-4782F88C2ACA}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>22.39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9.07</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6.7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6.11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6.01</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5.49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5.19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.07</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3.64</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3.6</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3.39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3.23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3.05</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3.05</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3.03</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2.83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2.09</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1.36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1.3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C50131-0DB7-684F-A025-B51B124079F9}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1057,324 +2824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07DDED0-8EB0-1747-9B54-4782F88C2ACA}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="32" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>22.39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>9.07</v>
-      </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6.7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6.11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6.01</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5.49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5.19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4.07</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="22" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3.64</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="22" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3.6</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>3.39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>3.23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>3.05</v>
-      </c>
-      <c r="B16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>3.05</v>
-      </c>
-      <c r="B17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>3.03</v>
-      </c>
-      <c r="B18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2.83</v>
-      </c>
-      <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2.09</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1.36</v>
-      </c>
-      <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1.3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8986C048-E3E5-7540-B0FF-4B08E5D1C8EA}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -1667,7 +3117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F67F30F-41AB-B74D-A197-51D2B0A81B76}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -2041,7 +3491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D432B1F4-6D1E-C247-BDF2-C7B4549B7C9B}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -2204,7 +3654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25286D2-7EFF-7B4F-A1E6-F81F6280D97E}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -2376,478 +3826,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159888AA-A2CB-E149-AEFC-0984670E0D56}">
-  <dimension ref="A1:D51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="37.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0.14888499999999999</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>9.8431000000000005E-2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>5.3726000000000003E-2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>5.2663000000000001E-2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4.7896000000000001E-2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>3.7117999999999998E-2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3.4874000000000002E-2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>2.9073999999999999E-2</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>2.8028999999999998E-2</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>2.6471000000000001E-2</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>2.5964000000000001E-2</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2.4220999999999999E-2</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>2.3806000000000001E-2</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>2.1336000000000001E-2</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1.7930000000000001E-2</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>1.7385999999999999E-2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1.4432E-2</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>1.37E-2</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>1.3213000000000001E-2</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>1.2843E-2</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>1.2788000000000001E-2</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>1.2095E-2</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>1.1764E-2</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>1.0971E-2</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>1.0614999999999999E-2</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>9.1190000000000004E-3</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>8.8669999999999999E-3</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>8.7849999999999994E-3</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>8.3149999999999995E-3</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>8.1309999999999993E-3</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>7.7980000000000002E-3</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>7.6969999999999998E-3</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>7.5950000000000002E-3</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>7.1310000000000002E-3</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>6.842E-3</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>6.6620000000000004E-3</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>6.5729999999999998E-3</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>6.5319999999999996E-3</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>6.3140000000000002E-3</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>6.2750000000000002E-3</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>6.0010000000000003E-3</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>5.9760000000000004E-3</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>5.7299999999999999E-3</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>5.6559999999999996E-3</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>5.3969999999999999E-3</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>4.7299999999999998E-3</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>4.5139999999999998E-3</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
-        <v>3.8349999999999999E-3</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
-        <v>3.7620000000000002E-3</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
-        <v>3.0990000000000002E-3</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>